<commit_message>
Ya se hizo el merge
</commit_message>
<xml_diff>
--- a/Acts/Integracion_Datos/tablas_todas_juntas.xlsx
+++ b/Acts/Integracion_Datos/tablas_todas_juntas.xlsx
@@ -5,22 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santl\PycharmProjects\Minero\MineriaDatos\Acts\Integracion_Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\- ITESO\- SEM 6\PROGRA MINERIA DATOS\MineriaDatos\Acts\Integracion_Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886F4EF3-4CF0-4011-BC5A-D2E3634340E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E65058-2D67-4C63-8B72-E7DAE5703BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add more data to your tables, I" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'add more data to your tables, I'!$H$1:$L$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="156">
   <si>
     <t>CustomerID</t>
   </si>
@@ -481,133 +497,19 @@
     <t>Address</t>
   </si>
   <si>
-    <t>123 Main Street</t>
-  </si>
-  <si>
-    <t>456 Oak Avenue</t>
-  </si>
-  <si>
-    <t>789 Pine Lane</t>
-  </si>
-  <si>
-    <t>999 Willow Drive</t>
-  </si>
-  <si>
-    <t>246 Maple Avenue</t>
-  </si>
-  <si>
-    <t>135 Cedar Lane</t>
-  </si>
-  <si>
-    <t>864 Birch Road</t>
-  </si>
-  <si>
-    <t>579 Spruce Street</t>
-  </si>
-  <si>
-    <t>258 Walnut Avenue</t>
-  </si>
-  <si>
-    <t>159 Cherry Lane</t>
-  </si>
-  <si>
-    <t>876 Hickory Road</t>
-  </si>
-  <si>
-    <t>581 Sycamore Street</t>
-  </si>
-  <si>
-    <t>263 Redwood Avenue</t>
-  </si>
-  <si>
-    <t>168 Oakwood Lane</t>
-  </si>
-  <si>
-    <t>794 Pinehurst Drive</t>
-  </si>
-  <si>
-    <t>279 Maplewood Avenue</t>
-  </si>
-  <si>
-    <t>148 Cedarcrest Lane</t>
-  </si>
-  <si>
-    <t>873 Birchwood Road</t>
-  </si>
-  <si>
-    <t>584 Sprucelawn Street</t>
-  </si>
-  <si>
-    <t>267 Walnutcrest Avenue</t>
-  </si>
-  <si>
-    <t>164 Cherrywood Lane</t>
-  </si>
-  <si>
-    <t>881 Hickorycrest Road</t>
-  </si>
-  <si>
-    <t>586 Sycamorelawn Street</t>
-  </si>
-  <si>
-    <t>268 Redwoodcrest Avenue</t>
-  </si>
-  <si>
-    <t>173 Oakwoodcrest Lane</t>
-  </si>
-  <si>
-    <t>799 Pinehurstcrest Drive</t>
-  </si>
-  <si>
-    <t>284 Maplewoodcrest Avenue</t>
-  </si>
-  <si>
-    <t>153 Cedarcrestcrest Lane</t>
-  </si>
-  <si>
-    <t>878 Birchwoodcrest Road</t>
-  </si>
-  <si>
-    <t>589 Sprucelawncrest Street</t>
-  </si>
-  <si>
-    <t>272 Walnutcrestcrest Avenue</t>
-  </si>
-  <si>
-    <t>169 Cherrywoodcrest Lane</t>
-  </si>
-  <si>
-    <t>886 Hickorycrestcrest Road</t>
-  </si>
-  <si>
-    <t>591 Sycamorelawncrest Street</t>
-  </si>
-  <si>
-    <t>274 Redwoodcrestcrest Avenue</t>
-  </si>
-  <si>
-    <t>179 Oakwoodcrestcrest Lane</t>
-  </si>
-  <si>
-    <t>804 Pinehurstcrestcrest Drive</t>
-  </si>
-  <si>
-    <t>289 Maplewoodcrestcrest Avenue</t>
-  </si>
-  <si>
-    <t>158 Cedarcrestcrestcrest Lane</t>
-  </si>
-  <si>
-    <t>883 Birchwoodcrestcrest Road</t>
+    <t>DIFERENCIA</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -648,10 +550,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -872,34 +773,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.21875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="5.44140625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.42578125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -945,21 +846,24 @@
       <c r="S1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="U1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1001</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>45591</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>125.5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="H2">
@@ -968,7 +872,7 @@
       <c r="I2" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>45591</v>
       </c>
       <c r="K2">
@@ -983,46 +887,46 @@
       <c r="P2" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>45061</v>
       </c>
       <c r="R2">
         <v>1500</v>
       </c>
       <c r="S2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>1002</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>45592</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>50</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="H3">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I3" t="s">
-        <v>112</v>
-      </c>
-      <c r="J3" s="3">
-        <v>45593</v>
+        <v>115</v>
+      </c>
+      <c r="J3" s="2">
+        <v>45592</v>
       </c>
       <c r="K3">
-        <v>195.5</v>
+        <v>49.99</v>
       </c>
       <c r="L3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O3">
         <v>1002</v>
@@ -1030,46 +934,46 @@
       <c r="P3" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="2">
         <v>45139</v>
       </c>
       <c r="R3">
         <v>800</v>
       </c>
       <c r="S3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>1003</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>45593</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>200.75</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="H4">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J4" s="3">
-        <v>45594</v>
+        <v>112</v>
+      </c>
+      <c r="J4" s="2">
+        <v>45593</v>
       </c>
       <c r="K4">
-        <v>90</v>
+        <v>195.5</v>
       </c>
       <c r="L4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="O4">
         <v>1003</v>
@@ -1077,46 +981,46 @@
       <c r="P4" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <v>45250</v>
       </c>
       <c r="R4">
         <v>2200</v>
       </c>
       <c r="S4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>1004</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2">
         <v>45593</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>75.25</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="H5">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="I5" t="s">
-        <v>115</v>
-      </c>
-      <c r="J5" s="3">
-        <v>45592</v>
+        <v>114</v>
+      </c>
+      <c r="J5" s="2">
+        <v>45594</v>
       </c>
       <c r="K5">
-        <v>49.99</v>
+        <v>90</v>
       </c>
       <c r="L5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="O5">
         <v>1006</v>
@@ -1124,30 +1028,30 @@
       <c r="P5" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <v>45301</v>
       </c>
       <c r="R5">
         <v>300</v>
       </c>
       <c r="S5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>1005</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>45594</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>90</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="H6">
@@ -1156,7 +1060,7 @@
       <c r="I6" t="s">
         <v>117</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>45595</v>
       </c>
       <c r="K6">
@@ -1171,30 +1075,30 @@
       <c r="P6" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="2">
         <v>45337</v>
       </c>
       <c r="R6">
         <v>450</v>
       </c>
       <c r="S6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>1006</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>45595</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>150</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
       <c r="H7">
@@ -1203,7 +1107,7 @@
       <c r="I7" t="s">
         <v>119</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>45596</v>
       </c>
       <c r="K7">
@@ -1218,30 +1122,30 @@
       <c r="P7" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="2">
         <v>45371</v>
       </c>
       <c r="R7">
         <v>600</v>
       </c>
       <c r="S7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>1007</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>45596</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>60.5</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
       <c r="H8">
@@ -1250,7 +1154,7 @@
       <c r="I8" t="s">
         <v>120</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>45597</v>
       </c>
       <c r="K8">
@@ -1265,30 +1169,30 @@
       <c r="P8" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="2">
         <v>45407</v>
       </c>
       <c r="R8">
         <v>750</v>
       </c>
       <c r="S8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>1008</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>45597</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>110.25</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="H9">
@@ -1297,7 +1201,7 @@
       <c r="I9" t="s">
         <v>121</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>45598</v>
       </c>
       <c r="K9">
@@ -1312,30 +1216,30 @@
       <c r="P9" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <v>45442</v>
       </c>
       <c r="R9">
         <v>900</v>
       </c>
       <c r="S9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>1009</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>45598</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>85</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>22</v>
       </c>
       <c r="H10">
@@ -1344,7 +1248,7 @@
       <c r="I10" t="s">
         <v>122</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>45599</v>
       </c>
       <c r="K10">
@@ -1359,30 +1263,30 @@
       <c r="P10" t="s">
         <v>25</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10" s="2">
         <v>45447</v>
       </c>
       <c r="R10">
         <v>1050</v>
       </c>
       <c r="S10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>1010</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="2">
         <v>45599</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>175.75</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>24</v>
       </c>
       <c r="H11">
@@ -1391,7 +1295,7 @@
       <c r="I11" t="s">
         <v>123</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>45600</v>
       </c>
       <c r="K11">
@@ -1406,30 +1310,30 @@
       <c r="P11" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11" s="2">
         <v>45482</v>
       </c>
       <c r="R11">
         <v>1200</v>
       </c>
       <c r="S11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>1011</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="2">
         <v>45600</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>95</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>26</v>
       </c>
       <c r="H12">
@@ -1438,7 +1342,7 @@
       <c r="I12" t="s">
         <v>124</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>45601</v>
       </c>
       <c r="K12">
@@ -1453,30 +1357,30 @@
       <c r="P12" t="s">
         <v>29</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12" s="2">
         <v>45518</v>
       </c>
       <c r="R12">
         <v>1350</v>
       </c>
       <c r="S12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>1012</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="2">
         <v>45601</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>135.25</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>28</v>
       </c>
       <c r="H13">
@@ -1485,7 +1389,7 @@
       <c r="I13" t="s">
         <v>125</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>45602</v>
       </c>
       <c r="K13">
@@ -1500,30 +1404,30 @@
       <c r="P13" t="s">
         <v>31</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="2">
         <v>45554</v>
       </c>
       <c r="R13">
         <v>1500</v>
       </c>
       <c r="S13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>1013</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="2">
         <v>45602</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>70</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>30</v>
       </c>
       <c r="H14">
@@ -1532,7 +1436,7 @@
       <c r="I14" t="s">
         <v>126</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>45603</v>
       </c>
       <c r="K14">
@@ -1547,30 +1451,30 @@
       <c r="P14" t="s">
         <v>33</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="2">
         <v>45589</v>
       </c>
       <c r="R14">
         <v>1650</v>
       </c>
       <c r="S14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>1014</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="2">
         <v>45603</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>120.5</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>32</v>
       </c>
       <c r="H15">
@@ -1579,7 +1483,7 @@
       <c r="I15" t="s">
         <v>127</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>45604</v>
       </c>
       <c r="K15">
@@ -1594,30 +1498,30 @@
       <c r="P15" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="2">
         <v>45593</v>
       </c>
       <c r="R15">
         <v>1800</v>
       </c>
       <c r="S15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>1015</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="2">
         <v>45604</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>100</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>34</v>
       </c>
       <c r="H16">
@@ -1626,7 +1530,7 @@
       <c r="I16" t="s">
         <v>128</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>45605</v>
       </c>
       <c r="K16">
@@ -1641,30 +1545,30 @@
       <c r="P16" t="s">
         <v>37</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16" s="2">
         <v>45598</v>
       </c>
       <c r="R16">
         <v>1950</v>
       </c>
       <c r="S16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>1016</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="2">
         <v>45605</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>160.75</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>36</v>
       </c>
       <c r="H17">
@@ -1673,7 +1577,7 @@
       <c r="I17" t="s">
         <v>129</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>45606</v>
       </c>
       <c r="K17">
@@ -1688,30 +1592,30 @@
       <c r="P17" t="s">
         <v>39</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="Q17" s="2">
         <v>45603</v>
       </c>
       <c r="R17">
         <v>2100</v>
       </c>
       <c r="S17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>1017</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="2">
         <v>45606</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>80</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>38</v>
       </c>
       <c r="H18">
@@ -1720,7 +1624,7 @@
       <c r="I18" t="s">
         <v>130</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>45607</v>
       </c>
       <c r="K18">
@@ -1735,30 +1639,30 @@
       <c r="P18" t="s">
         <v>41</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="Q18" s="2">
         <v>45608</v>
       </c>
       <c r="R18">
         <v>2250</v>
       </c>
       <c r="S18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>1018</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>45607</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>140.25</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>40</v>
       </c>
       <c r="H19">
@@ -1767,7 +1671,7 @@
       <c r="I19" t="s">
         <v>131</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>45608</v>
       </c>
       <c r="K19">
@@ -1782,30 +1686,30 @@
       <c r="P19" t="s">
         <v>43</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="Q19" s="2">
         <v>45613</v>
       </c>
       <c r="R19">
         <v>2400</v>
       </c>
       <c r="S19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>1019</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="2">
         <v>45608</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>115</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>42</v>
       </c>
       <c r="H20">
@@ -1814,7 +1718,7 @@
       <c r="I20" t="s">
         <v>132</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>45609</v>
       </c>
       <c r="K20">
@@ -1829,30 +1733,30 @@
       <c r="P20" t="s">
         <v>45</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20" s="2">
         <v>45618</v>
       </c>
       <c r="R20">
         <v>2550</v>
       </c>
       <c r="S20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>1020</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="2">
         <v>45609</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>90</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>44</v>
       </c>
       <c r="H21">
@@ -1861,7 +1765,7 @@
       <c r="I21" t="s">
         <v>133</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>45610</v>
       </c>
       <c r="K21">
@@ -1876,30 +1780,30 @@
       <c r="P21" t="s">
         <v>47</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21" s="2">
         <v>45623</v>
       </c>
       <c r="R21">
         <v>2700</v>
       </c>
       <c r="S21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>1021</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="2">
         <v>45610</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>180.75</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>46</v>
       </c>
       <c r="H22">
@@ -1908,7 +1812,7 @@
       <c r="I22" t="s">
         <v>134</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>45611</v>
       </c>
       <c r="K22">
@@ -1923,30 +1827,30 @@
       <c r="P22" t="s">
         <v>49</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22" s="2">
         <v>45628</v>
       </c>
       <c r="R22">
         <v>2850</v>
       </c>
       <c r="S22" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>1022</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="2">
         <v>45611</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>100</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>48</v>
       </c>
       <c r="H23">
@@ -1955,7 +1859,7 @@
       <c r="I23" t="s">
         <v>135</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>45612</v>
       </c>
       <c r="K23">
@@ -1970,30 +1874,30 @@
       <c r="P23" t="s">
         <v>51</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="Q23" s="2">
         <v>45633</v>
       </c>
       <c r="R23">
         <v>3000</v>
       </c>
       <c r="S23" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>1023</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="2">
         <v>45612</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>145.25</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>50</v>
       </c>
       <c r="H24">
@@ -2002,7 +1906,7 @@
       <c r="I24" t="s">
         <v>136</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <v>45613</v>
       </c>
       <c r="K24">
@@ -2017,30 +1921,30 @@
       <c r="P24" t="s">
         <v>53</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24" s="2">
         <v>45638</v>
       </c>
       <c r="R24">
         <v>3150</v>
       </c>
       <c r="S24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>1024</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="2">
         <v>45613</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>75</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>52</v>
       </c>
       <c r="H25">
@@ -2049,7 +1953,7 @@
       <c r="I25" t="s">
         <v>137</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>45614</v>
       </c>
       <c r="K25">
@@ -2064,30 +1968,30 @@
       <c r="P25" t="s">
         <v>55</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="Q25" s="2">
         <v>45643</v>
       </c>
       <c r="R25">
         <v>3300</v>
       </c>
       <c r="S25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>1025</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="2">
         <v>45614</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>125.5</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>54</v>
       </c>
       <c r="H26">
@@ -2096,7 +2000,7 @@
       <c r="I26" t="s">
         <v>138</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <v>45615</v>
       </c>
       <c r="K26">
@@ -2111,30 +2015,30 @@
       <c r="P26" t="s">
         <v>57</v>
       </c>
-      <c r="Q26" s="3">
+      <c r="Q26" s="2">
         <v>45648</v>
       </c>
       <c r="R26">
         <v>3450</v>
       </c>
       <c r="S26" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>1026</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="2">
         <v>45615</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>105</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>56</v>
       </c>
       <c r="H27">
@@ -2143,7 +2047,7 @@
       <c r="I27" t="s">
         <v>139</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <v>45616</v>
       </c>
       <c r="K27">
@@ -2158,30 +2062,30 @@
       <c r="P27" t="s">
         <v>59</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27" s="2">
         <v>45653</v>
       </c>
       <c r="R27">
         <v>3600</v>
       </c>
       <c r="S27" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>1027</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="2">
         <v>45616</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>165.75</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>58</v>
       </c>
       <c r="H28">
@@ -2190,7 +2094,7 @@
       <c r="I28" t="s">
         <v>140</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <v>45617</v>
       </c>
       <c r="K28">
@@ -2205,30 +2109,30 @@
       <c r="P28" t="s">
         <v>61</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28" s="2">
         <v>45658</v>
       </c>
       <c r="R28">
         <v>3750</v>
       </c>
       <c r="S28" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>1028</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="2">
         <v>45617</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>85</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>60</v>
       </c>
       <c r="H29">
@@ -2237,7 +2141,7 @@
       <c r="I29" t="s">
         <v>141</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <v>45618</v>
       </c>
       <c r="K29">
@@ -2252,30 +2156,30 @@
       <c r="P29" t="s">
         <v>63</v>
       </c>
-      <c r="Q29" s="3">
+      <c r="Q29" s="2">
         <v>45663</v>
       </c>
       <c r="R29">
         <v>3900</v>
       </c>
       <c r="S29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>1029</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="2">
         <v>45618</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>145.25</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>62</v>
       </c>
       <c r="H30">
@@ -2284,7 +2188,7 @@
       <c r="I30" t="s">
         <v>142</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <v>45619</v>
       </c>
       <c r="K30">
@@ -2299,30 +2203,30 @@
       <c r="P30" t="s">
         <v>65</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q30" s="2">
         <v>45668</v>
       </c>
       <c r="R30">
         <v>4050</v>
       </c>
       <c r="S30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>1030</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="2">
         <v>45619</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>120</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>64</v>
       </c>
       <c r="H31">
@@ -2331,7 +2235,7 @@
       <c r="I31" t="s">
         <v>143</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <v>45620</v>
       </c>
       <c r="K31">
@@ -2346,30 +2250,30 @@
       <c r="P31" t="s">
         <v>67</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q31" s="2">
         <v>45673</v>
       </c>
       <c r="R31">
         <v>4200</v>
       </c>
       <c r="S31" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>1031</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="2">
         <v>45620</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>95</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>66</v>
       </c>
       <c r="H32">
@@ -2378,7 +2282,7 @@
       <c r="I32" t="s">
         <v>144</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <v>45621</v>
       </c>
       <c r="K32">
@@ -2393,30 +2297,30 @@
       <c r="P32" t="s">
         <v>69</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="Q32" s="2">
         <v>45678</v>
       </c>
       <c r="R32">
         <v>4350</v>
       </c>
       <c r="S32" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>1032</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="2">
         <v>45621</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>185.75</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>68</v>
       </c>
       <c r="H33">
@@ -2425,7 +2329,7 @@
       <c r="I33" t="s">
         <v>145</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <v>45622</v>
       </c>
       <c r="K33">
@@ -2440,30 +2344,30 @@
       <c r="P33" t="s">
         <v>71</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="Q33" s="2">
         <v>45683</v>
       </c>
       <c r="R33">
         <v>4500</v>
       </c>
       <c r="S33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>1033</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>69</v>
       </c>
       <c r="C34" s="2">
         <v>45622</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>105</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>70</v>
       </c>
       <c r="H34">
@@ -2472,7 +2376,7 @@
       <c r="I34" t="s">
         <v>146</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <v>45623</v>
       </c>
       <c r="K34">
@@ -2487,30 +2391,30 @@
       <c r="P34" t="s">
         <v>73</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="Q34" s="2">
         <v>45688</v>
       </c>
       <c r="R34">
         <v>4650</v>
       </c>
       <c r="S34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>1034</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>71</v>
       </c>
       <c r="C35" s="2">
         <v>45623</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>150.25</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>72</v>
       </c>
       <c r="H35">
@@ -2519,74 +2423,78 @@
       <c r="I35" t="s">
         <v>147</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="2">
         <v>45624</v>
       </c>
       <c r="K35">
         <v>82</v>
       </c>
+      <c r="L35" t="s">
+        <v>154</v>
+      </c>
       <c r="O35">
         <v>1036</v>
       </c>
       <c r="P35" t="s">
         <v>75</v>
       </c>
-      <c r="Q35" s="3">
+      <c r="Q35" s="2">
         <v>45693</v>
       </c>
       <c r="R35">
         <v>4800</v>
       </c>
       <c r="S35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>1035</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>73</v>
       </c>
       <c r="C36" s="2">
         <v>45624</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>80</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>74</v>
       </c>
+      <c r="J36" s="2"/>
       <c r="O36">
         <v>1037</v>
       </c>
       <c r="P36" t="s">
         <v>77</v>
       </c>
-      <c r="Q36" s="3">
+      <c r="Q36" s="2">
         <v>45698</v>
       </c>
       <c r="R36">
         <v>4950</v>
       </c>
       <c r="S36" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>1036</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>75</v>
       </c>
       <c r="C37" s="2">
         <v>45625</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>130.5</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>76</v>
       </c>
       <c r="O37">
@@ -2595,30 +2503,30 @@
       <c r="P37" t="s">
         <v>79</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="Q37" s="2">
         <v>45703</v>
       </c>
       <c r="R37">
         <v>5100</v>
       </c>
       <c r="S37" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>1037</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>77</v>
       </c>
       <c r="C38" s="2">
         <v>45626</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38">
         <v>110</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>78</v>
       </c>
       <c r="O38">
@@ -2627,30 +2535,30 @@
       <c r="P38" t="s">
         <v>81</v>
       </c>
-      <c r="Q38" s="3">
+      <c r="Q38" s="2">
         <v>45708</v>
       </c>
       <c r="R38">
         <v>5250</v>
       </c>
       <c r="S38" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>1038</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="2">
         <v>45627</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39">
         <v>170.75</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>80</v>
       </c>
       <c r="O39">
@@ -2659,30 +2567,30 @@
       <c r="P39" t="s">
         <v>83</v>
       </c>
-      <c r="Q39" s="3">
+      <c r="Q39" s="2">
         <v>45713</v>
       </c>
       <c r="R39">
         <v>5400</v>
       </c>
       <c r="S39" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>1039</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>81</v>
       </c>
       <c r="C40" s="2">
         <v>45628</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40">
         <v>90</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>82</v>
       </c>
       <c r="O40">
@@ -2691,30 +2599,30 @@
       <c r="P40" t="s">
         <v>85</v>
       </c>
-      <c r="Q40" s="3">
+      <c r="Q40" s="2">
         <v>45718</v>
       </c>
       <c r="R40">
         <v>5550</v>
       </c>
       <c r="S40" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>1040</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>83</v>
       </c>
       <c r="C41" s="2">
         <v>45629</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41">
         <v>150.25</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>84</v>
       </c>
       <c r="O41">
@@ -2723,190 +2631,204 @@
       <c r="P41" t="s">
         <v>87</v>
       </c>
-      <c r="Q41" s="3">
+      <c r="Q41" s="2">
         <v>45723</v>
       </c>
       <c r="R41">
         <v>5700</v>
       </c>
       <c r="S41" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>1041</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="2">
         <v>45630</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42">
         <v>125</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>86</v>
       </c>
       <c r="O42">
         <v>1043</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="P42" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>154</v>
+      </c>
+      <c r="R42" t="s">
+        <v>154</v>
+      </c>
+      <c r="S42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>1042</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>87</v>
       </c>
       <c r="C43" s="2">
         <v>45631</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43">
         <v>100</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44">
         <v>1043</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>89</v>
       </c>
       <c r="C44" s="2">
         <v>45632</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44">
         <v>190.75</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="45" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>1044</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>91</v>
       </c>
       <c r="C45" s="2">
         <v>45633</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45">
         <v>110</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="46" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46">
         <v>1045</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>93</v>
       </c>
       <c r="C46" s="2">
         <v>45634</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46">
         <v>155.25</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+    <row r="47" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47">
         <v>1046</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>95</v>
       </c>
       <c r="C47" s="2">
         <v>45635</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47">
         <v>85</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="48" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48">
         <v>1047</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>97</v>
       </c>
       <c r="C48" s="2">
         <v>45636</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48">
         <v>135.5</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49">
         <v>1048</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>99</v>
       </c>
       <c r="C49" s="2">
         <v>45637</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49">
         <v>115</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50">
         <v>1049</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>101</v>
       </c>
       <c r="C50" s="2">
         <v>45638</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50">
         <v>175.75</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51">
         <v>1050</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>103</v>
       </c>
       <c r="C51" s="2">
         <v>45639</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51">
         <v>95</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="H1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>